<commit_message>
Refactor data handling and stuff
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Books" sheetId="1" state="visible" r:id="rId1"/>
@@ -396,8 +396,8 @@
   </sheetPr>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -486,7 +486,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Shaurya</t>
+          <t>NULL</t>
         </is>
       </c>
     </row>
@@ -741,8 +741,8 @@
   </sheetPr>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>

</xml_diff>